<commit_message>
update system send notification duplicated delegate exclusion
</commit_message>
<xml_diff>
--- a/storage/app/templates/delegates_template.xlsx
+++ b/storage/app/templates/delegates_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10203"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianexavier/Documents/Documents - Xavier’s MacBook Pro/A &amp; A Creation/Customer/CU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianexavier/Code/cuems/storage/app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E7D7C00-F82D-7B44-9A8B-202755698D14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA3DD9-F5AA-C14C-ACF3-4E992CE4DD54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>Title</t>
   </si>
@@ -220,6 +220,18 @@
   </si>
   <si>
     <t>Prof</t>
+  </si>
+  <si>
+    <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Cheque</t>
   </si>
 </sst>
 </file>
@@ -663,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -681,17 +693,17 @@
     <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="22.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="1" customWidth="1"/>
-    <col min="12" max="16" width="21.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="29.33203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="22.1640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="40.33203125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1640625" style="1"/>
+    <col min="12" max="17" width="21.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="22.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="29.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="22.1640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="40.33203125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,28 +750,31 @@
         <v>33</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -806,13 +821,16 @@
         <v>31</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
@@ -856,28 +874,31 @@
         <v>31</v>
       </c>
       <c r="P3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="4">
         <v>66281556</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -921,9 +942,12 @@
         <v>31</v>
       </c>
       <c r="P4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -932,7 +956,7 @@
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{1FFBC5EE-A2D2-AB45-8C48-4E12285868B8}"/>
-    <hyperlink ref="T3" r:id="rId3" xr:uid="{B76D5812-0F00-144A-B1F0-D3DD35A89A30}"/>
+    <hyperlink ref="U3" r:id="rId3" xr:uid="{B76D5812-0F00-144A-B1F0-D3DD35A89A30}"/>
     <hyperlink ref="L4" r:id="rId4" xr:uid="{1FF869A1-E7F4-404D-9FDC-2FBF8A816CE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>